<commit_message>
Script to plot protocols.
</commit_message>
<xml_diff>
--- a/Protocols/BehaviourProtocols.xlsx
+++ b/Protocols/BehaviourProtocols.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="55">
   <si>
     <t>CODE</t>
   </si>
@@ -52,7 +52,7 @@
     <t>NextProbeTrial-HIGH</t>
   </si>
   <si>
-    <t>Number of trials</t>
+    <t>NumTrialsInABlock</t>
   </si>
   <si>
     <t>Comments</t>
@@ -176,18 +176,6 @@
   </si>
   <si>
     <t>light + 750 trace + puff1</t>
-  </si>
-  <si>
-    <t>NOTES:</t>
-  </si>
-  <si>
-    <t>Camera trigger on for last 500ms of PreStim to first 500ms of PostStim</t>
-  </si>
-  <si>
-    <t>Probe:  Last trial of every block (4+probe).</t>
-  </si>
-  <si>
-    <t>puff1 is the usual US. puff2 is what Hrishi would need as a second US.</t>
   </si>
 </sst>
 </file>
@@ -262,7 +250,7 @@
     <col customWidth="1" min="9" max="10" width="21.86"/>
     <col customWidth="1" min="12" max="13" width="18.0"/>
     <col customWidth="1" min="14" max="14" width="19.43"/>
-    <col customWidth="1" min="15" max="15" width="63.14"/>
+    <col customWidth="1" min="15" max="15" width="34.86"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -311,6 +299,7 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="P1" s="1"/>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
@@ -971,27 +960,19 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="A18" s="3"/>
       <c r="B18" s="3"/>
     </row>
     <row r="19">
-      <c r="A19" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="A19" s="3"/>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
     </row>
     <row r="20">
-      <c r="A20" s="3" t="s">
-        <v>57</v>
-      </c>
+      <c r="A20" s="3"/>
     </row>
     <row r="21">
-      <c r="A21" s="3" t="s">
-        <v>58</v>
-      </c>
+      <c r="A21" s="3"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>